<commit_message>
06.07.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/July/Others/Price list June 2020.xlsx
+++ b/2020/July/Others/Price list June 2020.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="88">
   <si>
     <t>Model</t>
   </si>
@@ -276,9 +276,6 @@
     <t>D47</t>
   </si>
   <si>
-    <t>June</t>
-  </si>
-  <si>
     <t>BL120</t>
   </si>
   <si>
@@ -289,6 +286,12 @@
   </si>
   <si>
     <t>T180</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>Z30</t>
   </si>
 </sst>
 </file>
@@ -644,7 +647,7 @@
         <xdr:cNvPr id="2" name="Group 19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -665,7 +668,7 @@
           <xdr:cNvPr id="3" name="Freeform 21">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -871,7 +874,7 @@
           <xdr:cNvPr id="4" name="Freeform 22">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1972,7 +1975,7 @@
           <xdr:cNvPr id="5" name="Freeform 23">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2412,7 +2415,7 @@
           <xdr:cNvPr id="6" name="Freeform 24">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000006000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2472,7 +2475,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2489,7 +2492,7 @@
           <xdr:cNvPr id="7" name="Freeform 25">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000007000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2552,7 +2555,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2569,7 +2572,7 @@
           <xdr:cNvPr id="8" name="Freeform 26">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008000000}"/>
+                <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -2629,7 +2632,7 @@
           </a:ln>
           <a:extLst>
             <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-              <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+              <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2662,7 +2665,7 @@
         <xdr:cNvPr id="9" name="Picture 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000009000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2674,7 +2677,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -2952,7 +2955,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2962,8 +2965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="O36" sqref="O35:O36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3035,7 +3038,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="31" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="I4" s="31"/>
       <c r="J4" s="32">
@@ -3289,9 +3292,7 @@
       <c r="C13" s="6">
         <v>860</v>
       </c>
-      <c r="D13" s="6">
-        <v>45</v>
-      </c>
+      <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="7"/>
       <c r="G13" s="12" t="s">
@@ -3393,9 +3394,7 @@
       <c r="I16" s="8">
         <v>1290</v>
       </c>
-      <c r="J16" s="6">
-        <v>55</v>
-      </c>
+      <c r="J16" s="6"/>
       <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:11" ht="21.6" customHeight="1">
@@ -3408,9 +3407,7 @@
       <c r="C17" s="6">
         <v>910</v>
       </c>
-      <c r="D17" s="6">
-        <v>25</v>
-      </c>
+      <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="7"/>
       <c r="G17" s="12" t="s">
@@ -3422,9 +3419,7 @@
       <c r="I17" s="8">
         <v>1190</v>
       </c>
-      <c r="J17" s="6">
-        <v>45</v>
-      </c>
+      <c r="J17" s="6"/>
       <c r="K17" s="6"/>
     </row>
     <row r="18" spans="1:11" ht="21.6" customHeight="1">
@@ -3458,7 +3453,7 @@
     </row>
     <row r="19" spans="1:11" ht="21.6" customHeight="1">
       <c r="A19" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B19" s="6">
         <v>920</v>
@@ -3501,7 +3496,7 @@
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H20" s="8">
         <v>1220</v>
@@ -3806,7 +3801,7 @@
     </row>
     <row r="31" spans="1:11" ht="21.6" customHeight="1">
       <c r="A31" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B31" s="8">
         <v>4050</v>
@@ -4031,9 +4026,7 @@
       <c r="I38" s="8">
         <v>7990</v>
       </c>
-      <c r="J38" s="6">
-        <v>700</v>
-      </c>
+      <c r="J38" s="6"/>
       <c r="K38" s="6">
         <v>0</v>
       </c>
@@ -4112,13 +4105,13 @@
       </c>
       <c r="F41" s="7"/>
       <c r="G41" s="12" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="H41" s="8">
-        <v>8310</v>
+        <v>9300</v>
       </c>
       <c r="I41" s="8">
-        <v>8990</v>
+        <v>9790</v>
       </c>
       <c r="J41" s="6"/>
       <c r="K41" s="6">
@@ -4135,21 +4128,19 @@
       <c r="C42" s="8">
         <v>6990</v>
       </c>
-      <c r="D42" s="8">
-        <v>400</v>
-      </c>
+      <c r="D42" s="8"/>
       <c r="E42" s="6">
         <v>0</v>
       </c>
       <c r="F42" s="7"/>
       <c r="G42" s="12" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="H42" s="8">
-        <v>10340</v>
+        <v>8310</v>
       </c>
       <c r="I42" s="8">
-        <v>10990</v>
+        <v>8990</v>
       </c>
       <c r="J42" s="6"/>
       <c r="K42" s="6">
@@ -4163,11 +4154,19 @@
       <c r="D43" s="8"/>
       <c r="E43" s="6"/>
       <c r="F43" s="7"/>
-      <c r="G43" s="12"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
+      <c r="G43" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="H43" s="8">
+        <v>10340</v>
+      </c>
+      <c r="I43" s="8">
+        <v>10990</v>
+      </c>
       <c r="J43" s="6"/>
-      <c r="K43" s="6"/>
+      <c r="K43" s="6">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:12" ht="21.6" customHeight="1">
       <c r="A44" s="12"/>
@@ -4188,7 +4187,7 @@
       </c>
       <c r="B45" s="24"/>
       <c r="C45" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D45" s="27"/>
       <c r="E45" s="27"/>

</xml_diff>